<commit_message>
modificado stored procedure para truncar tablas históricas
</commit_message>
<xml_diff>
--- a/Archivos Origen/ReporteFinal/ReporteFinal.xlsx
+++ b/Archivos Origen/ReporteFinal/ReporteFinal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1e3f28d0bdc4dc07/Documentos/DemoSISS/Archivos Origen/ReporteFinal/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="14_{2FE81DE0-1847-4C37-8425-76278BF394E0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{AC3B1D8E-1DBD-445C-91DE-E052FEC9D916}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="14_{2FE81DE0-1847-4C37-8425-76278BF394E0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{248449A7-1D59-4B0F-A401-5E5A6E40196E}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0D99F8A8-7E31-44FC-A9C0-2973D025F3C7}"/>
   </bookViews>
@@ -400,7 +400,7 @@
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD4001"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -410,7 +410,7 @@
     <col min="3" max="3" width="35" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.88671875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.77734375" customWidth="1"/>
+    <col min="6" max="6" width="13.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -440,21 +440,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010028E59967AEA6194F96A8883902E1EAD2" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3506f466aa5c04d465c5c43c8d5a6502">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="e356fe65-c95c-4903-930e-2f989d172e03" xmlns:ns4="35410de1-fa75-40f3-901d-75599929c7bd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7eef5d787e73aeebfac4f4ad827faa24" ns3:_="" ns4:_="">
     <xsd:import namespace="e356fe65-c95c-4903-930e-2f989d172e03"/>
@@ -657,24 +642,22 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{98EA86A2-D81E-4BA0-959A-8C05E39F5A91}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4CC5F10B-CEDE-4EB3-8FA6-773D879C1D3F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{86B1F203-A23D-4693-963A-3DE6A5CFD039}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -691,4 +674,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4CC5F10B-CEDE-4EB3-8FA6-773D879C1D3F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{98EA86A2-D81E-4BA0-959A-8C05E39F5A91}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>